<commit_message>
Updated deps and fixed resulting async issues.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="10320" windowWidth="23070" xWindow="930" yWindow="0"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -350,6 +350,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for number formats.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -41,6 +41,7 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font/>
   </fonts>
   <fills>
     <fill>
@@ -58,12 +59,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf fontId="1" borderId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,6 +358,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored _SharedStrings a bit.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -41,7 +41,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font/>
   </fonts>
   <fills>
     <fill>
@@ -59,14 +58,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf fontId="1" borderId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,11 +355,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Work on style sheet tests.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -33,6 +33,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts/>
   <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -40,6 +41,9 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills>
@@ -58,12 +62,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf fontId="1" borderId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +357,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switched _ContentTypes to JSON.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -34,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts/>
-  <fonts x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,11 +42,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-    </font>
   </fonts>
-  <fills>
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -62,14 +59,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf fontId="1" borderId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +352,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switched _Relationships to JSON.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -34,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -51,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -63,7 +63,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>

<commit_message>
Large number of small changes.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -24,11 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>This is neat!</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,8 +348,19 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1">
+        <v>0.47568978777511184</v>
+      </c>
+      <c r="B1">
+        <v>0.21298007248749995</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0.3303780960716638</v>
+      </c>
+      <c r="B2">
+        <v>0.24623383579351343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up examples. Fixed new cells with row/column styles.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -24,7 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t>This is neat!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -348,19 +352,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>0.6959000800377888</v>
-      </c>
-      <c r="B1">
-        <v>0.018499864711871483</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>0.364119517286541</v>
-      </c>
-      <c r="B2">
-        <v>0.8607343968470482</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding/moving sheets. Tab colors.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\xlsx-populate\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\GitHub\xlsx-populate\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +29,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t xml:space="preserve">This is neat!</t>
+    <t xml:space="preserve">undefined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts/>
   <fonts x14ac:knownFonts="1">
     <font>
@@ -128,9 +131,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -158,14 +161,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -193,6 +213,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -345,13 +382,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -359,4 +418,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added reading error values and keeping stored formula values until writing.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -9,13 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12795"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="17475" windowHeight="7035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,10 +23,88 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>David Johnson</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Johnson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+C</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Script MT Bold"/>
+            <family val="4"/>
+          </rPr>
+          <t>o</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mple</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>x!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t xml:space="preserve">undefined</t>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Complex</t>
   </si>
 </sst>
 </file>
@@ -44,6 +119,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Script MT Bold"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills>
@@ -381,81 +482,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="e">
+        <f>1/B3</f>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue with lots of columns.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\GitHub\xlsx-populate\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\xlsx-populate\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="17475" windowHeight="7035"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,94 +23,16 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>David Johnson</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Comment</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>David Johnson:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-C</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Script MT Bold"/>
-            <family val="4"/>
-          </rPr>
-          <t>o</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>mple</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>x!</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Simple</t>
-  </si>
-  <si>
-    <t>Complex</t>
+    <t xml:space="preserve">This is neat!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts/>
   <fonts x14ac:knownFonts="1">
     <font>
@@ -119,32 +41,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Script MT Bold"/>
-      <family val="4"/>
     </font>
   </fonts>
   <fills>
@@ -232,9 +128,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -262,31 +158,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -314,23 +193,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -482,39 +344,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
-        <f>1/B3</f>
-      </c>
-      <c r="B3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More work on tests.
</commit_message>
<xml_diff>
--- a/examples/basic/out.xlsx
+++ b/examples/basic/out.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="foo" sheetId="2" r:id="rId5" state="hidden"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -348,7 +349,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -360,4 +361,14 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+</worksheet>
 </file>
</xml_diff>